<commit_message>
Atualiza├º├úo autom├ítica OEE, Canudos e Producao (19/01/2026 16:26:01,53)
</commit_message>
<xml_diff>
--- a/Canudos.xlsx
+++ b/Canudos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLANILHAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CEF40EB-72F5-47C4-BCCF-17E7FF7F3E32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89A0393-5B5E-4385-8BE3-43EF9B98B0C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2551C110-448D-4C8A-AC10-E46F4B669B16}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="67">
   <si>
     <t>OS</t>
   </si>
@@ -228,13 +228,13 @@
     <t>BRANCO COM AMARELO 177 (COR 649)</t>
   </si>
   <si>
-    <t>8524/8502</t>
-  </si>
-  <si>
-    <t>A/B</t>
-  </si>
-  <si>
     <t>PRODUÇÃO DE CANUDO BRANCO COM PROBLEMA NO ENCABEÇAMENTO</t>
+  </si>
+  <si>
+    <t>cor 475</t>
+  </si>
+  <si>
+    <t>canudo preto e branco</t>
   </si>
 </sst>
 </file>
@@ -1195,8 +1195,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>115381</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>824897</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>142438</xdr:rowOff>
     </xdr:to>
@@ -2137,17 +2137,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AA5261E-B2CC-424C-A60F-51E466D0160F}">
-  <dimension ref="A1:S89"/>
+  <dimension ref="A1:S92"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="J92" sqref="J92"/>
+      <selection activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.7109375" style="2" customWidth="1"/>
     <col min="2" max="6" width="19.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" style="1" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="15.28515625" style="1" customWidth="1"/>
     <col min="10" max="10" width="20.140625" style="1" customWidth="1"/>
@@ -2233,7 +2233,7 @@
       <c r="I2" s="13"/>
       <c r="J2" s="14">
         <f>AVERAGE(E2:E206)</f>
-        <v>8712.7816091954028</v>
+        <v>8679.393258426966</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>13</v>
@@ -2280,12 +2280,12 @@
       <c r="I3" s="12"/>
       <c r="K3" s="4">
         <f>SUM(E2:E2000)</f>
-        <v>758012</v>
+        <v>772466</v>
       </c>
       <c r="L3" s="4"/>
       <c r="M3" s="18">
         <f>SUM(F2:F2000)</f>
-        <v>4752</v>
+        <v>4790</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>27</v>
@@ -4281,19 +4281,70 @@
         <v>46038</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>64</v>
+        <v>6</v>
+      </c>
+      <c r="D89" s="1">
+        <v>8524</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="2">
+        <v>46038</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D90" s="1">
+        <v>8502</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="2">
+        <v>46039</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D91" s="1">
+        <v>8502</v>
+      </c>
+      <c r="E91" s="1">
+        <v>7454</v>
+      </c>
+      <c r="F91" s="1">
+        <v>17</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="2">
+        <v>46041</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D92" s="1">
+        <v>8524</v>
+      </c>
+      <c r="E92" s="1">
+        <v>7000</v>
+      </c>
+      <c r="F92" s="1">
+        <v>21</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualiza├º├úo autom├ítica OEE, Canudos e Producao (20/01/2026  8:15:07,89)
</commit_message>
<xml_diff>
--- a/Canudos.xlsx
+++ b/Canudos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLANILHAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89A0393-5B5E-4385-8BE3-43EF9B98B0C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EABC7CFA-9B89-4C1E-86EB-CB7EC47FEBF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2551C110-448D-4C8A-AC10-E46F4B669B16}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="68">
   <si>
     <t>OS</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>canudo preto e branco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cor 475 </t>
   </si>
 </sst>
 </file>
@@ -2137,10 +2140,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AA5261E-B2CC-424C-A60F-51E466D0160F}">
-  <dimension ref="A1:S92"/>
+  <dimension ref="A1:S94"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="D93" sqref="D93"/>
+      <selection activeCell="F94" sqref="F94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2233,7 +2236,7 @@
       <c r="I2" s="13"/>
       <c r="J2" s="14">
         <f>AVERAGE(E2:E206)</f>
-        <v>8679.393258426966</v>
+        <v>8585.1868131868123</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>13</v>
@@ -2280,12 +2283,12 @@
       <c r="I3" s="12"/>
       <c r="K3" s="4">
         <f>SUM(E2:E2000)</f>
-        <v>772466</v>
+        <v>781252</v>
       </c>
       <c r="L3" s="4"/>
       <c r="M3" s="18">
         <f>SUM(F2:F2000)</f>
-        <v>4790</v>
+        <v>4806</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>27</v>
@@ -4345,6 +4348,46 @@
       </c>
       <c r="G92" s="1" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="2">
+        <v>46041</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D93" s="1">
+        <v>8502</v>
+      </c>
+      <c r="E93" s="1">
+        <v>1777</v>
+      </c>
+      <c r="F93" s="1">
+        <v>0</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="2">
+        <v>46041</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C94" s="1">
+        <v>1406169</v>
+      </c>
+      <c r="D94" s="1">
+        <v>8502</v>
+      </c>
+      <c r="E94" s="1">
+        <v>7009</v>
+      </c>
+      <c r="F94" s="1">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualiza├º├úo autom├ítica OEE, Canudos, Producao e Rejeito (23/01/2026  8:15:07,83)
</commit_message>
<xml_diff>
--- a/Canudos.xlsx
+++ b/Canudos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLANILHAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D63604F9-AAFD-46E5-AA43-8ABB48087F01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F3E866A-998C-42D2-97DF-84FD1B40AA1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2551C110-448D-4C8A-AC10-E46F4B669B16}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="69">
   <si>
     <t>OS</t>
   </si>
@@ -238,6 +238,9 @@
   </si>
   <si>
     <t xml:space="preserve">cor 475 </t>
+  </si>
+  <si>
+    <t>TREINAMENTO DE MAQUINA</t>
   </si>
 </sst>
 </file>
@@ -2140,10 +2143,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AA5261E-B2CC-424C-A60F-51E466D0160F}">
-  <dimension ref="A1:S96"/>
+  <dimension ref="A1:S98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D16" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2236,7 +2239,7 @@
       <c r="I2" s="13"/>
       <c r="J2" s="14">
         <f>AVERAGE(E2:E206)</f>
-        <v>8579.6989247311831</v>
+        <v>8561.1263157894737</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>13</v>
@@ -2283,12 +2286,12 @@
       <c r="I3" s="12"/>
       <c r="K3" s="4">
         <f>SUM(E2:E2000)</f>
-        <v>797912</v>
+        <v>813307</v>
       </c>
       <c r="L3" s="4"/>
       <c r="M3" s="18">
         <f>SUM(F2:F2000)</f>
-        <v>4855</v>
+        <v>4867</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>27</v>
@@ -4431,6 +4434,49 @@
       </c>
       <c r="F96" s="1">
         <v>12</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" s="2">
+        <v>46044</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C97" s="1">
+        <v>1406169</v>
+      </c>
+      <c r="D97" s="1">
+        <v>8524</v>
+      </c>
+      <c r="E97" s="1">
+        <v>9500</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" s="2">
+        <v>46044</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C98" s="1">
+        <v>1406169</v>
+      </c>
+      <c r="D98" s="1">
+        <v>8502</v>
+      </c>
+      <c r="E98" s="1">
+        <v>5895</v>
+      </c>
+      <c r="F98" s="1">
+        <v>12</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualiza├º├úo autom├ítica OEE, Canudos, Producao e Rejeito (24/01/2026  8:15:06,84)
</commit_message>
<xml_diff>
--- a/Canudos.xlsx
+++ b/Canudos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLANILHAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F3E866A-998C-42D2-97DF-84FD1B40AA1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF366CE-0CA1-46F3-8507-24BA9B235A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2551C110-448D-4C8A-AC10-E46F4B669B16}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="70">
   <si>
     <t>OS</t>
   </si>
@@ -241,6 +241,9 @@
   </si>
   <si>
     <t>TREINAMENTO DE MAQUINA</t>
+  </si>
+  <si>
+    <t>NÃO HOUVE PRODUÇÃO, AGUARDANDO MANUTENÇÃO DA MAQUINA</t>
   </si>
 </sst>
 </file>
@@ -2143,10 +2146,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AA5261E-B2CC-424C-A60F-51E466D0160F}">
-  <dimension ref="A1:S98"/>
+  <dimension ref="A1:S99"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A67" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="D92" sqref="D92"/>
+      <selection activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4436,7 +4439,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>46044</v>
       </c>
@@ -4456,7 +4459,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>46044</v>
       </c>
@@ -4477,6 +4480,26 @@
       </c>
       <c r="G98" s="1" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99" s="2">
+        <v>46045</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D99" s="1">
+        <v>8524</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H99" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualiza├º├úo autom├ítica OEE, Canudos, Producao e Rejeito (27/01/2026  8:15:06,60)
</commit_message>
<xml_diff>
--- a/Canudos.xlsx
+++ b/Canudos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLANILHAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF366CE-0CA1-46F3-8507-24BA9B235A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220D8826-7F32-4D05-9458-22778EC7C644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2551C110-448D-4C8A-AC10-E46F4B669B16}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="71">
   <si>
     <t>OS</t>
   </si>
@@ -244,6 +244,9 @@
   </si>
   <si>
     <t>NÃO HOUVE PRODUÇÃO, AGUARDANDO MANUTENÇÃO DA MAQUINA</t>
+  </si>
+  <si>
+    <t>MANUTENÇÃO CONCLUÍDA POR VOLTA DAS 10:30, OPERADOR FICOU NAS MAQUINAS E PASSANDO PRIMER POIS O HORÁRIO JÁ ESTAVA PRÓXIMO AO DO ALMOÇO</t>
   </si>
 </sst>
 </file>
@@ -2146,10 +2149,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AA5261E-B2CC-424C-A60F-51E466D0160F}">
-  <dimension ref="A1:S99"/>
+  <dimension ref="A1:S102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="A101" sqref="A101"/>
+    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="F102" sqref="F102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2242,7 +2245,7 @@
       <c r="I2" s="13"/>
       <c r="J2" s="14">
         <f>AVERAGE(E2:E206)</f>
-        <v>8561.1263157894737</v>
+        <v>8597.9583333333339</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>13</v>
@@ -2289,12 +2292,12 @@
       <c r="I3" s="12"/>
       <c r="K3" s="4">
         <f>SUM(E2:E2000)</f>
-        <v>813307</v>
+        <v>825404</v>
       </c>
       <c r="L3" s="4"/>
       <c r="M3" s="18">
         <f>SUM(F2:F2000)</f>
-        <v>4867</v>
+        <v>4877</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>27</v>
@@ -4500,6 +4503,66 @@
       </c>
       <c r="H99" s="1" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100" s="2">
+        <v>46046</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D100" s="1">
+        <v>8524</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G100" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H100" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A101" s="2">
+        <v>46048</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D101" s="1">
+        <v>8524</v>
+      </c>
+      <c r="F101" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G101" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H101" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102" s="2">
+        <v>46048</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C102" s="1">
+        <v>1406169</v>
+      </c>
+      <c r="D102" s="1">
+        <v>8502</v>
+      </c>
+      <c r="E102" s="1">
+        <v>12097</v>
+      </c>
+      <c r="F102" s="1">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualiza├º├úo autom├ítica OEE, Canudos, Producao e Rejeito (30/01/2026  8:15:06,74)
</commit_message>
<xml_diff>
--- a/Canudos.xlsx
+++ b/Canudos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLANILHAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220D8826-7F32-4D05-9458-22778EC7C644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE39568-5C6B-4543-AD2A-7C3A1CB9658C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2551C110-448D-4C8A-AC10-E46F4B669B16}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="74">
   <si>
     <t>OS</t>
   </si>
@@ -195,12 +195,6 @@
     <t>LILÁS ESMALTE</t>
   </si>
   <si>
-    <t>RAFAEL</t>
-  </si>
-  <si>
-    <t>VITINHO</t>
-  </si>
-  <si>
     <t>NOME</t>
   </si>
   <si>
@@ -247,6 +241,21 @@
   </si>
   <si>
     <t>MANUTENÇÃO CONCLUÍDA POR VOLTA DAS 10:30, OPERADOR FICOU NAS MAQUINAS E PASSANDO PRIMER POIS O HORÁRIO JÁ ESTAVA PRÓXIMO AO DO ALMOÇO</t>
+  </si>
+  <si>
+    <t>PEREIRA / MANUTENÇÃO</t>
+  </si>
+  <si>
+    <t>VITINHO / CANUDOS</t>
+  </si>
+  <si>
+    <t>RAFAEL / AUTOMAÇÃO</t>
+  </si>
+  <si>
+    <t>OPERADOR DIVIDIU O TEMPO ENTRE A MAQUINA DE CANUDOS E A DE IMPRESSÃO PARA AJUDAS NA PRODUÇÃO DE COPOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NÃO HOUVE PRODUÇÃO, OPERADOR FICOU NAS MAQUINAS 180/181 ENQUANTO OS OPERADORES MATHEUS E DIEGO FICARAM RODADANDO COPOS DE CAFÉ NA 28/182 PARA DOBRAR A PRODUÇÃO </t>
   </si>
 </sst>
 </file>
@@ -470,19 +479,15 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -553,10 +558,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1842,8 +1853,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{1FE77D6E-600C-406D-AA64-535CF7AD02D9}" name="Tabela4" displayName="Tabela4" ref="R2:S4" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11">
-  <autoFilter ref="R2:S4" xr:uid="{1FE77D6E-600C-406D-AA64-535CF7AD02D9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{1FE77D6E-600C-406D-AA64-535CF7AD02D9}" name="Tabela4" displayName="Tabela4" ref="R2:S5" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11">
+  <autoFilter ref="R2:S5" xr:uid="{1FE77D6E-600C-406D-AA64-535CF7AD02D9}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{065934BB-F4F9-47CC-8C25-186E2F5FD276}" name="NOME" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{5F9476BD-3CB7-480B-BA25-725A0FDEB9A9}" name="RAMAL" dataDxfId="8"/>
@@ -2149,10 +2160,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AA5261E-B2CC-424C-A60F-51E466D0160F}">
-  <dimension ref="A1:S102"/>
+  <dimension ref="A1:S106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="F102" sqref="F102"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="E107" sqref="E107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2166,7 +2177,7 @@
     <col min="11" max="13" width="14.5703125" style="1" customWidth="1"/>
     <col min="14" max="16" width="27.140625" style="1" customWidth="1"/>
     <col min="17" max="17" width="21.42578125" style="1" customWidth="1"/>
-    <col min="18" max="19" width="20.42578125" style="1" customWidth="1"/>
+    <col min="18" max="19" width="22.5703125" style="1" customWidth="1"/>
     <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -2201,11 +2212,11 @@
       <c r="J1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="K1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
       <c r="N1" s="15" t="s">
         <v>24</v>
       </c>
@@ -2216,12 +2227,12 @@
         <v>26</v>
       </c>
       <c r="Q1" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="R1" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="S1" s="28"/>
+        <v>55</v>
+      </c>
+      <c r="R1" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="S1" s="30"/>
     </row>
     <row r="2" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
@@ -2245,7 +2256,7 @@
       <c r="I2" s="13"/>
       <c r="J2" s="14">
         <f>AVERAGE(E2:E206)</f>
-        <v>8597.9583333333339</v>
+        <v>8529.3333333333339</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>13</v>
@@ -2263,11 +2274,11 @@
       <c r="P2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="R2" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="S2" s="25" t="s">
-        <v>56</v>
+      <c r="R2" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="S2" s="27" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -2292,12 +2303,12 @@
       <c r="I3" s="12"/>
       <c r="K3" s="4">
         <f>SUM(E2:E2000)</f>
-        <v>825404</v>
+        <v>844404</v>
       </c>
       <c r="L3" s="4"/>
       <c r="M3" s="18">
         <f>SUM(F2:F2000)</f>
-        <v>4877</v>
+        <v>4922</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>27</v>
@@ -2312,7 +2323,7 @@
         <v>1406169</v>
       </c>
       <c r="R3" s="20" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="S3" s="21">
         <v>4874</v>
@@ -2350,10 +2361,10 @@
       <c r="P4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="R4" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="S4" s="23">
+      <c r="R4" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="S4" s="25">
         <v>4991</v>
       </c>
     </row>
@@ -2385,6 +2396,12 @@
       <c r="P5" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="R5" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="S5" s="23">
+        <v>4979</v>
+      </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -3996,7 +4013,7 @@
         <v>37</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H74" s="1" t="s">
         <v>17</v>
@@ -4019,7 +4036,7 @@
         <v>54</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -4039,7 +4056,7 @@
         <v>23</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H76" s="1" t="s">
         <v>17</v>
@@ -4262,7 +4279,7 @@
         <v>26</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H87" s="1" t="s">
         <v>17</v>
@@ -4285,7 +4302,7 @@
         <v>72</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H88" s="1" t="s">
         <v>17</v>
@@ -4305,7 +4322,7 @@
         <v>17</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>17</v>
@@ -4339,7 +4356,7 @@
         <v>17</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -4359,7 +4376,7 @@
         <v>21</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
@@ -4379,7 +4396,7 @@
         <v>0</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -4459,7 +4476,7 @@
         <v>9500</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -4482,7 +4499,7 @@
         <v>12</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
@@ -4499,7 +4516,7 @@
         <v>17</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H99" s="1" t="s">
         <v>17</v>
@@ -4519,7 +4536,7 @@
         <v>17</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H100" s="1" t="s">
         <v>17</v>
@@ -4539,7 +4556,7 @@
         <v>17</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H101" s="1" t="s">
         <v>17</v>
@@ -4563,6 +4580,98 @@
       </c>
       <c r="F102" s="1">
         <v>10</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103" s="2">
+        <v>46049</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C103" s="1">
+        <v>1406169</v>
+      </c>
+      <c r="D103" s="1">
+        <v>8524</v>
+      </c>
+      <c r="E103" s="1">
+        <v>6200</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G103" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H103" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104" s="2">
+        <v>46050</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D104" s="1">
+        <v>8524</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G104" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A105" s="2">
+        <v>46050</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C105" s="1">
+        <v>1406169</v>
+      </c>
+      <c r="D105" s="1">
+        <v>8502</v>
+      </c>
+      <c r="E105" s="1">
+        <v>6795</v>
+      </c>
+      <c r="F105" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A106" s="2">
+        <v>46051</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C106" s="1">
+        <v>1406169</v>
+      </c>
+      <c r="D106" s="1">
+        <v>8524</v>
+      </c>
+      <c r="E106" s="1">
+        <v>6005</v>
+      </c>
+      <c r="F106" s="1">
+        <v>30</v>
+      </c>
+      <c r="G106" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H106" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualiza├º├úo autom├ítica OEE, Canudos, Producao e Rejeito (03/02/2026  8:15:07,32)
</commit_message>
<xml_diff>
--- a/Canudos.xlsx
+++ b/Canudos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLANILHAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE39568-5C6B-4543-AD2A-7C3A1CB9658C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A44ADC2A-2A4D-4677-9160-3C476A9DADD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2551C110-448D-4C8A-AC10-E46F4B669B16}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="75">
   <si>
     <t>OS</t>
   </si>
@@ -256,6 +256,9 @@
   </si>
   <si>
     <t xml:space="preserve">NÃO HOUVE PRODUÇÃO, OPERADOR FICOU NAS MAQUINAS 180/181 ENQUANTO OS OPERADORES MATHEUS E DIEGO FICARAM RODADANDO COPOS DE CAFÉ NA 28/182 PARA DOBRAR A PRODUÇÃO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAQUINA COM PROBLEMA NO CILINDRO DE PRESSÃO, APÓS CILINDRO BAIXAR, OS CANUDOS FICAM GRUDADOS NELE, ACARRETANDO EM UMA SOBREPOSILÇÃO NO CICLO SEGUINTE </t>
   </si>
 </sst>
 </file>
@@ -2160,10 +2163,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AA5261E-B2CC-424C-A60F-51E466D0160F}">
-  <dimension ref="A1:S106"/>
+  <dimension ref="A1:S107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="E107" sqref="E107"/>
+    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="A115" sqref="A115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2256,7 +2259,7 @@
       <c r="I2" s="13"/>
       <c r="J2" s="14">
         <f>AVERAGE(E2:E206)</f>
-        <v>8529.3333333333339</v>
+        <v>8458.0400000000009</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>13</v>
@@ -2303,12 +2306,12 @@
       <c r="I3" s="12"/>
       <c r="K3" s="4">
         <f>SUM(E2:E2000)</f>
-        <v>844404</v>
+        <v>845804</v>
       </c>
       <c r="L3" s="4"/>
       <c r="M3" s="18">
         <f>SUM(F2:F2000)</f>
-        <v>4922</v>
+        <v>4942</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>27</v>
@@ -4459,7 +4462,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>46044</v>
       </c>
@@ -4479,7 +4482,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
         <v>46044</v>
       </c>
@@ -4502,7 +4505,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
         <v>46045</v>
       </c>
@@ -4522,7 +4525,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>46046</v>
       </c>
@@ -4542,7 +4545,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
         <v>46048</v>
       </c>
@@ -4562,7 +4565,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
         <v>46048</v>
       </c>
@@ -4582,7 +4585,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
         <v>46049</v>
       </c>
@@ -4608,7 +4611,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
         <v>46050</v>
       </c>
@@ -4628,7 +4631,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
         <v>46050</v>
       </c>
@@ -4648,7 +4651,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
         <v>46051</v>
       </c>
@@ -4671,6 +4674,32 @@
         <v>72</v>
       </c>
       <c r="H106" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107" s="2">
+        <v>46053</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D107" s="1">
+        <v>8524</v>
+      </c>
+      <c r="E107" s="1">
+        <v>1400</v>
+      </c>
+      <c r="F107" s="1">
+        <v>20</v>
+      </c>
+      <c r="G107" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H107" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I107" s="1" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualiza├º├úo autom├ítica OEE, Canudos, Producao e Rejeito (06/02/2026 14:10:13,65)
</commit_message>
<xml_diff>
--- a/Canudos.xlsx
+++ b/Canudos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLANILHAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A44ADC2A-2A4D-4677-9160-3C476A9DADD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC41DEE5-7763-4A5F-8558-1C987DD2E77B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2551C110-448D-4C8A-AC10-E46F4B669B16}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="77">
   <si>
     <t>OS</t>
   </si>
@@ -259,6 +259,12 @@
   </si>
   <si>
     <t xml:space="preserve">MAQUINA COM PROBLEMA NO CILINDRO DE PRESSÃO, APÓS CILINDRO BAIXAR, OS CANUDOS FICAM GRUDADOS NELE, ACARRETANDO EM UMA SOBREPOSILÇÃO NO CICLO SEGUINTE </t>
+  </si>
+  <si>
+    <t>MAQUINA APRESENTOU PROBLEMA NA QUEDA DE CANUDOS  DA CALHA PARA A CORRENTE, TENTIVA DE MANUTENÇÃO POR OPERADOR RESPONSAVEL</t>
+  </si>
+  <si>
+    <t>PROBLEMA ENCONTRADO, PORÉM, APENAS AUTOMAÇÃO PODE RESOLVER, OPERDOR LIGOU PARA O RESPONSAVEL DA MAQUINA NA AUTOMAÇÃO MAS O MESMO ESTAVA AFASTADO NO DIA POR ATESDADO</t>
   </si>
 </sst>
 </file>
@@ -2163,10 +2169,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AA5261E-B2CC-424C-A60F-51E466D0160F}">
-  <dimension ref="A1:S107"/>
+  <dimension ref="A1:S110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="A115" sqref="A115"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="J120" sqref="J120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2259,7 +2265,7 @@
       <c r="I2" s="13"/>
       <c r="J2" s="14">
         <f>AVERAGE(E2:E206)</f>
-        <v>8458.0400000000009</v>
+        <v>8435.4752475247533</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>13</v>
@@ -2306,12 +2312,12 @@
       <c r="I3" s="12"/>
       <c r="K3" s="4">
         <f>SUM(E2:E2000)</f>
-        <v>845804</v>
+        <v>851983</v>
       </c>
       <c r="L3" s="4"/>
       <c r="M3" s="18">
         <f>SUM(F2:F2000)</f>
-        <v>4942</v>
+        <v>4967</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>27</v>
@@ -4700,6 +4706,69 @@
         <v>17</v>
       </c>
       <c r="I107" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108" s="2">
+        <v>46056</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D108" s="1">
+        <v>8502</v>
+      </c>
+      <c r="E108" s="1">
+        <v>6179</v>
+      </c>
+      <c r="F108" s="1">
+        <v>25</v>
+      </c>
+      <c r="G108" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109" s="2">
+        <v>46057</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D109" s="1">
+        <v>8524</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G109" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H109" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110" s="2">
+        <v>46058</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D110" s="1">
+        <v>8524</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G110" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I110" s="1" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualiza├º├úo autom├ítica OEE, Canudos, Producao e Rejeito (07/02/2026  8:15:07,26)
</commit_message>
<xml_diff>
--- a/Canudos.xlsx
+++ b/Canudos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLANILHAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC41DEE5-7763-4A5F-8558-1C987DD2E77B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D814FFCC-0592-4714-A15A-9D26E68225BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2551C110-448D-4C8A-AC10-E46F4B669B16}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="78">
   <si>
     <t>OS</t>
   </si>
@@ -265,6 +265,9 @@
   </si>
   <si>
     <t>PROBLEMA ENCONTRADO, PORÉM, APENAS AUTOMAÇÃO PODE RESOLVER, OPERDOR LIGOU PARA O RESPONSAVEL DA MAQUINA NA AUTOMAÇÃO MAS O MESMO ESTAVA AFASTADO NO DIA POR ATESDADO</t>
+  </si>
+  <si>
+    <t>RESPONSAVEL PELA MANUTENÇÃO DA MAQUINA PERMANECE DE ATESTADO POR TEMPO INDETERMINADO, SIGO AGUARDANDO A MANUTENÇÃO</t>
   </si>
 </sst>
 </file>
@@ -2169,10 +2172,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AA5261E-B2CC-424C-A60F-51E466D0160F}">
-  <dimension ref="A1:S110"/>
+  <dimension ref="A1:S111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="J120" sqref="J120"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="A112" sqref="A112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4772,6 +4775,29 @@
         <v>17</v>
       </c>
     </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A111" s="2">
+        <v>46059</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D111" s="1">
+        <v>8524</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G111" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H111" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I111" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="K1:M1"/>

</xml_diff>

<commit_message>
Atualiza├º├úo autom├ítica OEE, Canudos, Producao e Rejeito (11/02/2026  8:15:05,91)
</commit_message>
<xml_diff>
--- a/Canudos.xlsx
+++ b/Canudos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLANILHAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D814FFCC-0592-4714-A15A-9D26E68225BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0919994-3114-4004-ABE1-5571F1E61078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2551C110-448D-4C8A-AC10-E46F4B669B16}"/>
+    <workbookView xWindow="2895" yWindow="2895" windowWidth="21600" windowHeight="11295" xr2:uid="{2551C110-448D-4C8A-AC10-E46F4B669B16}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="79">
   <si>
     <t>OS</t>
   </si>
@@ -268,6 +268,9 @@
   </si>
   <si>
     <t>RESPONSAVEL PELA MANUTENÇÃO DA MAQUINA PERMANECE DE ATESTADO POR TEMPO INDETERMINADO, SIGO AGUARDANDO A MANUTENÇÃO</t>
+  </si>
+  <si>
+    <t>cor 648</t>
   </si>
 </sst>
 </file>
@@ -2172,10 +2175,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AA5261E-B2CC-424C-A60F-51E466D0160F}">
-  <dimension ref="A1:S111"/>
+  <dimension ref="A1:S113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="A112" sqref="A112"/>
+    <sheetView tabSelected="1" topLeftCell="K37" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="G113" sqref="G113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2268,7 +2271,7 @@
       <c r="I2" s="13"/>
       <c r="J2" s="14">
         <f>AVERAGE(E2:E206)</f>
-        <v>8435.4752475247533</v>
+        <v>8317.5922330097092</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>13</v>
@@ -2315,12 +2318,12 @@
       <c r="I3" s="12"/>
       <c r="K3" s="4">
         <f>SUM(E2:E2000)</f>
-        <v>851983</v>
+        <v>856712</v>
       </c>
       <c r="L3" s="4"/>
       <c r="M3" s="18">
         <f>SUM(F2:F2000)</f>
-        <v>4967</v>
+        <v>5012</v>
       </c>
       <c r="N3" s="1" t="s">
         <v>27</v>
@@ -4796,6 +4799,46 @@
       </c>
       <c r="I111" s="1" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A112" s="2">
+        <v>46063</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D112" s="1">
+        <v>8502</v>
+      </c>
+      <c r="E112" s="1">
+        <v>2650</v>
+      </c>
+      <c r="F112" s="1">
+        <v>35</v>
+      </c>
+      <c r="G112" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" s="2">
+        <v>46063</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D113" s="1">
+        <v>8502</v>
+      </c>
+      <c r="E113" s="1">
+        <v>2079</v>
+      </c>
+      <c r="F113" s="1">
+        <v>10</v>
+      </c>
+      <c r="G113" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualiza├º├úo autom├ítica OEE, Canudos, Producao e Rejeito (12/02/2026  8:15:06,63)
</commit_message>
<xml_diff>
--- a/Canudos.xlsx
+++ b/Canudos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLANILHAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0919994-3114-4004-ABE1-5571F1E61078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F6E1C4-9E64-48C5-98B5-8F9F90A059EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2895" yWindow="2895" windowWidth="21600" windowHeight="11295" xr2:uid="{2551C110-448D-4C8A-AC10-E46F4B669B16}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2551C110-448D-4C8A-AC10-E46F4B669B16}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="80">
   <si>
     <t>OS</t>
   </si>
@@ -271,6 +271,9 @@
   </si>
   <si>
     <t>cor 648</t>
+  </si>
+  <si>
+    <t>MAQUINA VOLTA A APRESENTAR DEFEITO NA ENGRENAGEM QUE JOGA OS CANUDOS DA CALHA PARA A ESTEIRA, RAPHAEL DA AUTOMAÇÃO LEVOU O EIXO POR COMPLETO PARA MANUTENÇÃO, AGUARDANDO RETORNO</t>
   </si>
 </sst>
 </file>
@@ -601,31 +604,6 @@
   <dxfs count="33">
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -777,6 +755,31 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1228,13 +1231,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1210562</xdr:colOff>
+      <xdr:colOff>1599338</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>824897</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>95943</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>142438</xdr:rowOff>
     </xdr:to>
@@ -1265,8 +1268,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9097262" y="0"/>
-          <a:ext cx="1324169" cy="828238"/>
+          <a:off x="9472042" y="0"/>
+          <a:ext cx="1324947" cy="832515"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1841,38 +1844,38 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5BB2D3F9-C887-4B4C-B99D-D2DF65DEC2A6}" name="Tabela5" displayName="Tabela5" ref="A1:H1048576" totalsRowCount="1" headerRowDxfId="32" dataDxfId="30" headerRowBorderDxfId="31">
   <autoFilter ref="A1:H1048575" xr:uid="{5BB2D3F9-C887-4B4C-B99D-D2DF65DEC2A6}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{087A0113-3A7F-4ED4-85E5-B6DA7A785E6E}" name="Data" dataDxfId="29" totalsRowDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{B5ACDCB9-111C-4EEF-A7F2-0DFD4B46F701}" name="Turno" dataDxfId="28" totalsRowDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{8DF57E4B-CE5D-4D81-A024-AF995D46B0D6}" name="OS" dataDxfId="27" totalsRowDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{ED2D14F5-1612-4387-8474-BB902D6983C6}" name="Operador" dataDxfId="26" totalsRowDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{98386C95-9775-4F1F-A3CC-9A16E030AF66}" name="Produzidos" dataDxfId="25" totalsRowDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{3F049097-8486-4DDD-93F7-CCC691CC4860}" name="Perdas" dataDxfId="24" totalsRowDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{26B92E51-FF95-433C-9069-C56C7828476A}" name="Observação" dataDxfId="23" totalsRowDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{8B43B335-323F-4C61-82F4-07648230810B}" name="Coluna1" dataDxfId="22" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{087A0113-3A7F-4ED4-85E5-B6DA7A785E6E}" name="Data" dataDxfId="29" totalsRowDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{B5ACDCB9-111C-4EEF-A7F2-0DFD4B46F701}" name="Turno" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{8DF57E4B-CE5D-4D81-A024-AF995D46B0D6}" name="OS" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{ED2D14F5-1612-4387-8474-BB902D6983C6}" name="Operador" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{98386C95-9775-4F1F-A3CC-9A16E030AF66}" name="Produzidos" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{3F049097-8486-4DDD-93F7-CCC691CC4860}" name="Perdas" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{26B92E51-FF95-433C-9069-C56C7828476A}" name="Observação" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{8B43B335-323F-4C61-82F4-07648230810B}" name="Coluna1" dataDxfId="15" totalsRowDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89285ECA-F282-4F01-A009-CC89A51CDC7A}" name="Tabela1" displayName="Tabela1" ref="N1:Q27" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89285ECA-F282-4F01-A009-CC89A51CDC7A}" name="Tabela1" displayName="Tabela1" ref="N1:Q27" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12">
   <autoFilter ref="N1:Q27" xr:uid="{89285ECA-F282-4F01-A009-CC89A51CDC7A}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{EDE6611D-5889-4C5E-8516-947DDEFF7DCC}" name="CANUDOS " totalsRowLabel="Total" dataDxfId="18" totalsRowDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{7D1A3E97-C617-4FD2-B05B-A97B6AD5F90C}" name="CORES" dataDxfId="16" totalsRowDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{03E79F60-8E38-46EF-92B4-918A623037DE}" name="DESCRIÇÃO" totalsRowFunction="count" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{1B33BBDF-2D4E-45C0-873F-D04B114DCBBF}" name="os" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{EDE6611D-5889-4C5E-8516-947DDEFF7DCC}" name="CANUDOS " totalsRowLabel="Total" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{7D1A3E97-C617-4FD2-B05B-A97B6AD5F90C}" name="CORES" dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{03E79F60-8E38-46EF-92B4-918A623037DE}" name="DESCRIÇÃO" totalsRowFunction="count" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{1B33BBDF-2D4E-45C0-873F-D04B114DCBBF}" name="os" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{1FE77D6E-600C-406D-AA64-535CF7AD02D9}" name="Tabela4" displayName="Tabela4" ref="R2:S5" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{1FE77D6E-600C-406D-AA64-535CF7AD02D9}" name="Tabela4" displayName="Tabela4" ref="R2:S5" totalsRowShown="0" headerRowDxfId="4" dataDxfId="2" headerRowBorderDxfId="3">
   <autoFilter ref="R2:S5" xr:uid="{1FE77D6E-600C-406D-AA64-535CF7AD02D9}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{065934BB-F4F9-47CC-8C25-186E2F5FD276}" name="NOME" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{5F9476BD-3CB7-480B-BA25-725A0FDEB9A9}" name="RAMAL" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{065934BB-F4F9-47CC-8C25-186E2F5FD276}" name="NOME" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{5F9476BD-3CB7-480B-BA25-725A0FDEB9A9}" name="RAMAL" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2175,10 +2178,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AA5261E-B2CC-424C-A60F-51E466D0160F}">
-  <dimension ref="A1:S113"/>
+  <dimension ref="A1:S114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K37" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="G113" sqref="G113"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4821,7 +4824,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
         <v>46063</v>
       </c>
@@ -4839,6 +4842,26 @@
       </c>
       <c r="G113" s="1" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A114" s="2">
+        <v>46064</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D114" s="1">
+        <v>8524</v>
+      </c>
+      <c r="F114" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G114" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H114" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualiza├º├úo autom├ítica OEE, Canudos, Producao e Rejeito (12/02/2026 17:30:02,99)
</commit_message>
<xml_diff>
--- a/Canudos.xlsx
+++ b/Canudos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLANILHAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F6E1C4-9E64-48C5-98B5-8F9F90A059EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46149CEE-D66D-4D89-B85A-F45CD49DD8FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2551C110-448D-4C8A-AC10-E46F4B669B16}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="81">
   <si>
     <t>OS</t>
   </si>
@@ -274,6 +274,9 @@
   </si>
   <si>
     <t>MAQUINA VOLTA A APRESENTAR DEFEITO NA ENGRENAGEM QUE JOGA OS CANUDOS DA CALHA PARA A ESTEIRA, RAPHAEL DA AUTOMAÇÃO LEVOU O EIXO POR COMPLETO PARA MANUTENÇÃO, AGUARDANDO RETORNO</t>
+  </si>
+  <si>
+    <t>MAQUINA APRESENTOU PROBLEMA NA CONRRENTE DURANTE O TURNO B, AUTOMAÇÃO FOI CHAMADA, PORÉM, APENAS MANUTENÇÃO CONSEGUE MEXER, AGUARDANDO RETORNO DE RESPONSAVEL</t>
   </si>
 </sst>
 </file>
@@ -604,6 +607,31 @@
   <dxfs count="33">
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -755,31 +783,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1844,38 +1847,38 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5BB2D3F9-C887-4B4C-B99D-D2DF65DEC2A6}" name="Tabela5" displayName="Tabela5" ref="A1:H1048576" totalsRowCount="1" headerRowDxfId="32" dataDxfId="30" headerRowBorderDxfId="31">
   <autoFilter ref="A1:H1048575" xr:uid="{5BB2D3F9-C887-4B4C-B99D-D2DF65DEC2A6}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{087A0113-3A7F-4ED4-85E5-B6DA7A785E6E}" name="Data" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{B5ACDCB9-111C-4EEF-A7F2-0DFD4B46F701}" name="Turno" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{8DF57E4B-CE5D-4D81-A024-AF995D46B0D6}" name="OS" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{ED2D14F5-1612-4387-8474-BB902D6983C6}" name="Operador" dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{98386C95-9775-4F1F-A3CC-9A16E030AF66}" name="Produzidos" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{3F049097-8486-4DDD-93F7-CCC691CC4860}" name="Perdas" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{26B92E51-FF95-433C-9069-C56C7828476A}" name="Observação" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="8" xr3:uid="{8B43B335-323F-4C61-82F4-07648230810B}" name="Coluna1" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{087A0113-3A7F-4ED4-85E5-B6DA7A785E6E}" name="Data" dataDxfId="29" totalsRowDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{B5ACDCB9-111C-4EEF-A7F2-0DFD4B46F701}" name="Turno" dataDxfId="28" totalsRowDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{8DF57E4B-CE5D-4D81-A024-AF995D46B0D6}" name="OS" dataDxfId="27" totalsRowDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{ED2D14F5-1612-4387-8474-BB902D6983C6}" name="Operador" dataDxfId="26" totalsRowDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{98386C95-9775-4F1F-A3CC-9A16E030AF66}" name="Produzidos" dataDxfId="25" totalsRowDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{3F049097-8486-4DDD-93F7-CCC691CC4860}" name="Perdas" dataDxfId="24" totalsRowDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{26B92E51-FF95-433C-9069-C56C7828476A}" name="Observação" dataDxfId="23" totalsRowDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{8B43B335-323F-4C61-82F4-07648230810B}" name="Coluna1" dataDxfId="22" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89285ECA-F282-4F01-A009-CC89A51CDC7A}" name="Tabela1" displayName="Tabela1" ref="N1:Q27" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89285ECA-F282-4F01-A009-CC89A51CDC7A}" name="Tabela1" displayName="Tabela1" ref="N1:Q27" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20">
   <autoFilter ref="N1:Q27" xr:uid="{89285ECA-F282-4F01-A009-CC89A51CDC7A}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{EDE6611D-5889-4C5E-8516-947DDEFF7DCC}" name="CANUDOS " totalsRowLabel="Total" dataDxfId="10" totalsRowDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{7D1A3E97-C617-4FD2-B05B-A97B6AD5F90C}" name="CORES" dataDxfId="8" totalsRowDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{03E79F60-8E38-46EF-92B4-918A623037DE}" name="DESCRIÇÃO" totalsRowFunction="count" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{1B33BBDF-2D4E-45C0-873F-D04B114DCBBF}" name="os" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{EDE6611D-5889-4C5E-8516-947DDEFF7DCC}" name="CANUDOS " totalsRowLabel="Total" dataDxfId="18" totalsRowDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{7D1A3E97-C617-4FD2-B05B-A97B6AD5F90C}" name="CORES" dataDxfId="16" totalsRowDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{03E79F60-8E38-46EF-92B4-918A623037DE}" name="DESCRIÇÃO" totalsRowFunction="count" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{1B33BBDF-2D4E-45C0-873F-D04B114DCBBF}" name="os" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{1FE77D6E-600C-406D-AA64-535CF7AD02D9}" name="Tabela4" displayName="Tabela4" ref="R2:S5" totalsRowShown="0" headerRowDxfId="4" dataDxfId="2" headerRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{1FE77D6E-600C-406D-AA64-535CF7AD02D9}" name="Tabela4" displayName="Tabela4" ref="R2:S5" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11">
   <autoFilter ref="R2:S5" xr:uid="{1FE77D6E-600C-406D-AA64-535CF7AD02D9}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{065934BB-F4F9-47CC-8C25-186E2F5FD276}" name="NOME" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{5F9476BD-3CB7-480B-BA25-725A0FDEB9A9}" name="RAMAL" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{065934BB-F4F9-47CC-8C25-186E2F5FD276}" name="NOME" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{5F9476BD-3CB7-480B-BA25-725A0FDEB9A9}" name="RAMAL" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2178,10 +2181,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AA5261E-B2CC-424C-A60F-51E466D0160F}">
-  <dimension ref="A1:S114"/>
+  <dimension ref="A1:S115"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="G115" sqref="G115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4864,6 +4867,26 @@
         <v>17</v>
       </c>
     </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A115" s="2">
+        <v>46065</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D115" s="1">
+        <v>8524</v>
+      </c>
+      <c r="F115" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G115" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H115" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="K1:M1"/>

</xml_diff>

<commit_message>
Atualiza├º├úo autom├ítica (13/02/2026  8:15:06,07)
</commit_message>
<xml_diff>
--- a/Canudos.xlsx
+++ b/Canudos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLANILHAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46149CEE-D66D-4D89-B85A-F45CD49DD8FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D597524-ACA1-451F-94B5-3DD2ED876FC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2551C110-448D-4C8A-AC10-E46F4B669B16}"/>
+    <workbookView xWindow="2895" yWindow="2895" windowWidth="21600" windowHeight="11295" xr2:uid="{2551C110-448D-4C8A-AC10-E46F4B669B16}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="82">
   <si>
     <t>OS</t>
   </si>
@@ -277,6 +277,9 @@
   </si>
   <si>
     <t>MAQUINA APRESENTOU PROBLEMA NA CONRRENTE DURANTE O TURNO B, AUTOMAÇÃO FOI CHAMADA, PORÉM, APENAS MANUTENÇÃO CONSEGUE MEXER, AGUARDANDO RETORNO DE RESPONSAVEL</t>
+  </si>
+  <si>
+    <t>EMPRESA INTEIRA COM QUEDAS DE ENERGIA, PRESSÃO DAS MAQUINAS PRATICAMENTE NO ZERO</t>
   </si>
 </sst>
 </file>
@@ -2181,10 +2184,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AA5261E-B2CC-424C-A60F-51E466D0160F}">
-  <dimension ref="A1:S115"/>
+  <dimension ref="A1:S116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="G115" sqref="G115"/>
+    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="I113" sqref="I113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4887,6 +4890,26 @@
         <v>17</v>
       </c>
     </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A116" s="2">
+        <v>46065</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D116" s="1">
+        <v>8524</v>
+      </c>
+      <c r="F116" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G116" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H116" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="K1:M1"/>

</xml_diff>

<commit_message>
Atualiza├º├úo autom├ítica (14/02/2026  8:15:08,09)
</commit_message>
<xml_diff>
--- a/Canudos.xlsx
+++ b/Canudos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLANILHAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D597524-ACA1-451F-94B5-3DD2ED876FC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3D1318-5888-47FD-A0DF-6C50CE37206B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2895" yWindow="2895" windowWidth="21600" windowHeight="11295" xr2:uid="{2551C110-448D-4C8A-AC10-E46F4B669B16}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="83">
   <si>
     <t>OS</t>
   </si>
@@ -280,6 +280,9 @@
   </si>
   <si>
     <t>EMPRESA INTEIRA COM QUEDAS DE ENERGIA, PRESSÃO DAS MAQUINAS PRATICAMENTE NO ZERO</t>
+  </si>
+  <si>
+    <t>APENAS DOIS OPERADORES NO DIA, FIQUEI RODANDO AS MAQUINAS COM O DIEGUINHO, MATHUES NÃO VEIO POR CAUSA DO HORARIO COMERCIAL</t>
   </si>
 </sst>
 </file>
@@ -2184,10 +2187,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AA5261E-B2CC-424C-A60F-51E466D0160F}">
-  <dimension ref="A1:S116"/>
+  <dimension ref="A1:S118"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A99" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="I113" sqref="I113"/>
+      <selection activeCell="A118" sqref="A118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4910,6 +4913,40 @@
         <v>17</v>
       </c>
     </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A117" s="2">
+        <v>46066</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D117" s="1">
+        <v>8524</v>
+      </c>
+      <c r="G117" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A118" s="2">
+        <v>46067</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D118" s="1">
+        <v>8524</v>
+      </c>
+      <c r="F118" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G118" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H118" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="K1:M1"/>

</xml_diff>

<commit_message>
Atualiza├º├úo autom├ítica (16/02/2026 10:13:02,27)
</commit_message>
<xml_diff>
--- a/Canudos.xlsx
+++ b/Canudos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLANILHAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3D1318-5888-47FD-A0DF-6C50CE37206B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68A8C03-129B-4A40-BA39-C3BB64DFA8A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2895" yWindow="2895" windowWidth="21600" windowHeight="11295" xr2:uid="{2551C110-448D-4C8A-AC10-E46F4B669B16}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2551C110-448D-4C8A-AC10-E46F4B669B16}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -2190,7 +2190,7 @@
   <dimension ref="A1:S118"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A99" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="A118" sqref="A118"/>
+      <selection activeCell="A119" sqref="A119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Atualiza├º├úo autom├ítica (19/02/2026  8:15:06,85)
</commit_message>
<xml_diff>
--- a/Canudos.xlsx
+++ b/Canudos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PLANILHAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68A8C03-129B-4A40-BA39-C3BB64DFA8A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8727C2DF-832B-46CF-8B78-99DE78EAAB52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2551C110-448D-4C8A-AC10-E46F4B669B16}"/>
+    <workbookView xWindow="2895" yWindow="2895" windowWidth="21600" windowHeight="11295" xr2:uid="{2551C110-448D-4C8A-AC10-E46F4B669B16}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="83">
   <si>
     <t>OS</t>
   </si>
@@ -2187,10 +2187,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AA5261E-B2CC-424C-A60F-51E466D0160F}">
-  <dimension ref="A1:S118"/>
+  <dimension ref="A1:S119"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A99" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="A119" sqref="A119"/>
+      <selection activeCell="E112" sqref="E112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4947,6 +4947,20 @@
         <v>17</v>
       </c>
     </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A119" s="2">
+        <v>46071</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D119" s="1">
+        <v>8524</v>
+      </c>
+      <c r="G119" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="K1:M1"/>

</xml_diff>